<commit_message>
catch at length code and minor updates
I started creating the catch-at-length distribution that will enter the model. I also updated the data schedule to reflect the new discards size data I received.
</commit_message>
<xml_diff>
--- a/docs/data schedule for FY2026.xlsx
+++ b/docs/data schedule for FY2026.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.carr-harris\Desktop\Git\flukeRDM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEF2B5B-7AB8-4B40-A5AD-2C1A51754906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F84D0E-D76C-4E73-B37D-9EFCCE835270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D8E79F77-1C25-49C9-A795-4A01B72CB574}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D8E79F77-1C25-49C9-A795-4A01B72CB574}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t xml:space="preserve">  ALS - I have this</t>
   </si>
   <si>
-    <t xml:space="preserve">  Connecticut VAS</t>
-  </si>
-  <si>
     <t xml:space="preserve">  MRIP  - I have this</t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t xml:space="preserve">  Mass. VAS - program does not exist anymore for fluke, sea bass, and scup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Connecticut VAS - I have this</t>
   </si>
 </sst>
 </file>
@@ -320,6 +320,69 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -332,42 +395,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -375,33 +402,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -726,7 +726,7 @@
   <dimension ref="A2:AO33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,134 +735,134 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="20" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="20" t="s">
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="21"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="20" t="s">
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="34"/>
+      <c r="AA2" s="34"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="AD2" s="21"/>
-      <c r="AE2" s="21"/>
-      <c r="AF2" s="21"/>
-      <c r="AG2" s="21"/>
-      <c r="AH2" s="21"/>
-      <c r="AI2" s="21"/>
-      <c r="AJ2" s="21"/>
-      <c r="AK2" s="21"/>
-      <c r="AL2" s="21"/>
-      <c r="AM2" s="21"/>
-      <c r="AN2" s="22"/>
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="34"/>
+      <c r="AF2" s="34"/>
+      <c r="AG2" s="34"/>
+      <c r="AH2" s="34"/>
+      <c r="AI2" s="34"/>
+      <c r="AJ2" s="34"/>
+      <c r="AK2" s="34"/>
+      <c r="AL2" s="34"/>
+      <c r="AM2" s="34"/>
+      <c r="AN2" s="35"/>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19" t="s">
+      <c r="F3" s="24"/>
+      <c r="G3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19" t="s">
+      <c r="H3" s="24"/>
+      <c r="I3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19" t="s">
+      <c r="L3" s="24"/>
+      <c r="M3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19" t="s">
+      <c r="N3" s="24"/>
+      <c r="O3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19" t="s">
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19" t="s">
+      <c r="R3" s="24"/>
+      <c r="S3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19" t="s">
+      <c r="T3" s="24"/>
+      <c r="U3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="V3" s="19"/>
-      <c r="W3" s="19" t="s">
+      <c r="V3" s="24"/>
+      <c r="W3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="19" t="s">
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="19"/>
+      <c r="Z3" s="24"/>
       <c r="AA3" s="9"/>
       <c r="AB3" s="9"/>
-      <c r="AC3" s="19" t="s">
+      <c r="AC3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="AD3" s="19"/>
-      <c r="AE3" s="19" t="s">
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="AF3" s="19"/>
-      <c r="AG3" s="19" t="s">
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="AH3" s="19"/>
-      <c r="AI3" s="19" t="s">
+      <c r="AH3" s="24"/>
+      <c r="AI3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="AJ3" s="19"/>
-      <c r="AK3" s="19" t="s">
+      <c r="AJ3" s="24"/>
+      <c r="AK3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AL3" s="19"/>
-      <c r="AM3" s="19" t="s">
+      <c r="AL3" s="24"/>
+      <c r="AM3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="AN3" s="19"/>
+      <c r="AN3" s="24"/>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
@@ -987,96 +987,96 @@
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="29"/>
-      <c r="Z5" s="30"/>
-      <c r="AA5" s="26" t="s">
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="31"/>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="31"/>
+      <c r="Z5" s="32"/>
+      <c r="AA5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="AB5" s="27"/>
-      <c r="AC5" s="23" t="s">
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="AD5" s="24"/>
-      <c r="AE5" s="24"/>
-      <c r="AF5" s="24"/>
-      <c r="AG5" s="24"/>
-      <c r="AH5" s="24"/>
-      <c r="AI5" s="24"/>
-      <c r="AJ5" s="24"/>
-      <c r="AK5" s="24"/>
-      <c r="AL5" s="24"/>
-      <c r="AM5" s="24"/>
-      <c r="AN5" s="25"/>
+      <c r="AD5" s="26"/>
+      <c r="AE5" s="26"/>
+      <c r="AF5" s="26"/>
+      <c r="AG5" s="26"/>
+      <c r="AH5" s="26"/>
+      <c r="AI5" s="26"/>
+      <c r="AJ5" s="26"/>
+      <c r="AK5" s="26"/>
+      <c r="AL5" s="26"/>
+      <c r="AM5" s="26"/>
+      <c r="AN5" s="27"/>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="34" t="s">
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-      <c r="X6" s="35"/>
-      <c r="Y6" s="35"/>
-      <c r="Z6" s="35"/>
-      <c r="AA6" s="36"/>
-      <c r="AB6" s="37"/>
-      <c r="AC6" s="38" t="s">
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="AD6" s="36"/>
-      <c r="AE6" s="36"/>
-      <c r="AF6" s="36"/>
-      <c r="AG6" s="36"/>
-      <c r="AH6" s="36"/>
-      <c r="AI6" s="36"/>
-      <c r="AJ6" s="36"/>
-      <c r="AK6" s="36"/>
-      <c r="AL6" s="36"/>
-      <c r="AM6" s="36"/>
-      <c r="AN6" s="37"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="16"/>
+      <c r="AF6" s="16"/>
+      <c r="AG6" s="16"/>
+      <c r="AH6" s="16"/>
+      <c r="AI6" s="16"/>
+      <c r="AJ6" s="16"/>
+      <c r="AK6" s="16"/>
+      <c r="AL6" s="16"/>
+      <c r="AM6" s="16"/>
+      <c r="AN6" s="17"/>
       <c r="AO6" s="1"/>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.3">
@@ -1084,20 +1084,20 @@
       <c r="B7" s="2"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="41"/>
-      <c r="P7" s="42"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="23"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
@@ -1129,20 +1129,20 @@
       <c r="B8" s="2"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="33"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="42"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
@@ -1173,34 +1173,34 @@
       <c r="B9" s="2"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="15" t="s">
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="16"/>
-      <c r="AB9" s="17"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="37"/>
+      <c r="X9" s="37"/>
+      <c r="Y9" s="37"/>
+      <c r="Z9" s="37"/>
+      <c r="AA9" s="37"/>
+      <c r="AB9" s="38"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
       <c r="AE9" s="7"/>
@@ -1347,20 +1347,20 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
@@ -1442,7 +1442,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -1536,7 +1536,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
@@ -1600,7 +1600,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="13" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
@@ -1632,7 +1632,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
@@ -1664,7 +1664,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
@@ -1696,7 +1696,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="E27" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -1754,7 +1754,7 @@
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="E29" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="E30" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
@@ -1800,7 +1800,7 @@
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="E32" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
@@ -1816,7 +1816,7 @@
     </row>
     <row r="33" spans="5:16" x14ac:dyDescent="0.3">
       <c r="E33" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
@@ -1832,6 +1832,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="E9:P9"/>
+    <mergeCell ref="Q9:AB9"/>
+    <mergeCell ref="E13:P13"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E2:P2"/>
+    <mergeCell ref="E8:P8"/>
+    <mergeCell ref="Q6:AB6"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="C5:Z5"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="AC2:AN2"/>
+    <mergeCell ref="Q2:AB2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="AC6:AN6"/>
     <mergeCell ref="E6:P6"/>
     <mergeCell ref="E7:P7"/>
@@ -1848,24 +1866,6 @@
     <mergeCell ref="AC5:AN5"/>
     <mergeCell ref="AA5:AB5"/>
     <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="C5:Z5"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="AC2:AN2"/>
-    <mergeCell ref="Q2:AB2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="E9:P9"/>
-    <mergeCell ref="Q9:AB9"/>
-    <mergeCell ref="E13:P13"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E2:P2"/>
-    <mergeCell ref="E8:P8"/>
-    <mergeCell ref="Q6:AB6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
removed and updated pre_sim files and docs
updated the copula modeling loop - seems to work now without errors. updated the data schedule doc. created slides for TC meeting on 6_20. generated the baseline catch-at-length distribution. dropped some obsolete presim files. updated the catch-per-trip presim code.
</commit_message>
<xml_diff>
--- a/docs/data schedule for FY2026.xlsx
+++ b/docs/data schedule for FY2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.carr-harris\Desktop\Git\flukeRDM\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F84D0E-D76C-4E73-B37D-9EFCCE835270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4129D5-64C8-481A-8E90-C8F4BFAFAB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D8E79F77-1C25-49C9-A795-4A01B72CB574}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>w6</t>
   </si>
@@ -296,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -306,7 +306,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -320,69 +319,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -395,6 +331,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -402,6 +350,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -725,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1171110-A2BA-426B-9475-953CE499A9CF}">
   <dimension ref="A2:AO33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AG18" sqref="AG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,348 +734,350 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="33" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="33" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="34"/>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="33" t="s">
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="21"/>
+      <c r="AC2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
-      <c r="AF2" s="34"/>
-      <c r="AG2" s="34"/>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="35"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="20"/>
+      <c r="AL2" s="20"/>
+      <c r="AM2" s="20"/>
+      <c r="AN2" s="21"/>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24" t="s">
+      <c r="F3" s="18"/>
+      <c r="G3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24" t="s">
+      <c r="H3" s="18"/>
+      <c r="I3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24" t="s">
+      <c r="J3" s="18"/>
+      <c r="K3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24" t="s">
+      <c r="L3" s="18"/>
+      <c r="M3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24" t="s">
+      <c r="N3" s="18"/>
+      <c r="O3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24" t="s">
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24" t="s">
+      <c r="R3" s="18"/>
+      <c r="S3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24" t="s">
+      <c r="T3" s="18"/>
+      <c r="U3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24" t="s">
+      <c r="V3" s="18"/>
+      <c r="W3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24" t="s">
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="24" t="s">
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="AD3" s="24"/>
-      <c r="AE3" s="24" t="s">
+      <c r="AD3" s="18"/>
+      <c r="AE3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="AF3" s="24"/>
-      <c r="AG3" s="24" t="s">
+      <c r="AF3" s="18"/>
+      <c r="AG3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="AH3" s="24"/>
-      <c r="AI3" s="24" t="s">
+      <c r="AH3" s="18"/>
+      <c r="AI3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="AJ3" s="24"/>
-      <c r="AK3" s="24" t="s">
+      <c r="AJ3" s="18"/>
+      <c r="AK3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="AL3" s="24"/>
-      <c r="AM3" s="24" t="s">
+      <c r="AL3" s="18"/>
+      <c r="AM3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="AN3" s="24"/>
+      <c r="AN3" s="18"/>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>45170</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>45200</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>45231</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>45261</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>45292</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>45323</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <v>45352</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <v>45383</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="10">
         <v>45413</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="10">
         <v>45444</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="10">
         <v>45474</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="10">
         <v>45505</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="10">
         <v>45536</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="10">
         <v>45566</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="10">
         <v>45597</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="10">
         <v>45627</v>
       </c>
-      <c r="Q4" s="11">
+      <c r="Q4" s="10">
         <v>45658</v>
       </c>
-      <c r="R4" s="11">
+      <c r="R4" s="10">
         <v>45689</v>
       </c>
-      <c r="S4" s="11">
+      <c r="S4" s="10">
         <v>45717</v>
       </c>
-      <c r="T4" s="11">
+      <c r="T4" s="10">
         <v>45748</v>
       </c>
-      <c r="U4" s="11">
+      <c r="U4" s="10">
         <v>45778</v>
       </c>
-      <c r="V4" s="11">
+      <c r="V4" s="10">
         <v>45809</v>
       </c>
-      <c r="W4" s="11">
+      <c r="W4" s="10">
         <v>45839</v>
       </c>
-      <c r="X4" s="11">
+      <c r="X4" s="10">
         <v>45870</v>
       </c>
-      <c r="Y4" s="11">
+      <c r="Y4" s="10">
         <v>45901</v>
       </c>
-      <c r="Z4" s="11">
+      <c r="Z4" s="10">
         <v>45931</v>
       </c>
-      <c r="AA4" s="11">
+      <c r="AA4" s="10">
         <v>45962</v>
       </c>
-      <c r="AB4" s="11">
+      <c r="AB4" s="10">
         <v>45992</v>
       </c>
-      <c r="AC4" s="11">
+      <c r="AC4" s="10">
         <v>46023</v>
       </c>
-      <c r="AD4" s="11">
+      <c r="AD4" s="10">
         <v>46054</v>
       </c>
-      <c r="AE4" s="11">
+      <c r="AE4" s="10">
         <v>46082</v>
       </c>
-      <c r="AF4" s="11">
+      <c r="AF4" s="10">
         <v>46113</v>
       </c>
-      <c r="AG4" s="11">
+      <c r="AG4" s="10">
         <v>46143</v>
       </c>
-      <c r="AH4" s="11">
+      <c r="AH4" s="10">
         <v>46174</v>
       </c>
-      <c r="AI4" s="11">
+      <c r="AI4" s="10">
         <v>46204</v>
       </c>
-      <c r="AJ4" s="11">
+      <c r="AJ4" s="10">
         <v>46235</v>
       </c>
-      <c r="AK4" s="11">
+      <c r="AK4" s="10">
         <v>46266</v>
       </c>
-      <c r="AL4" s="11">
+      <c r="AL4" s="10">
         <v>46296</v>
       </c>
-      <c r="AM4" s="11">
+      <c r="AM4" s="10">
         <v>46327</v>
       </c>
-      <c r="AN4" s="11">
+      <c r="AN4" s="10">
         <v>46357</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="31"/>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="31"/>
-      <c r="Z5" s="32"/>
-      <c r="AA5" s="28" t="s">
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="30"/>
+      <c r="V5" s="30"/>
+      <c r="W5" s="30"/>
+      <c r="X5" s="30"/>
+      <c r="Y5" s="30"/>
+      <c r="Z5" s="31"/>
+      <c r="AA5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="AB5" s="29"/>
-      <c r="AC5" s="25" t="s">
+      <c r="AB5" s="41"/>
+      <c r="AC5" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="AD5" s="26"/>
-      <c r="AE5" s="26"/>
-      <c r="AF5" s="26"/>
-      <c r="AG5" s="26"/>
-      <c r="AH5" s="26"/>
-      <c r="AI5" s="26"/>
-      <c r="AJ5" s="26"/>
-      <c r="AK5" s="26"/>
-      <c r="AL5" s="26"/>
-      <c r="AM5" s="26"/>
-      <c r="AN5" s="27"/>
+      <c r="AD5" s="38"/>
+      <c r="AE5" s="38"/>
+      <c r="AF5" s="38"/>
+      <c r="AG5" s="38"/>
+      <c r="AH5" s="38"/>
+      <c r="AI5" s="38"/>
+      <c r="AJ5" s="38"/>
+      <c r="AK5" s="38"/>
+      <c r="AL5" s="38"/>
+      <c r="AM5" s="38"/>
+      <c r="AN5" s="39"/>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="18" t="s">
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="19"/>
-      <c r="V6" s="19"/>
-      <c r="W6" s="19"/>
-      <c r="X6" s="19"/>
-      <c r="Y6" s="19"/>
-      <c r="Z6" s="19"/>
-      <c r="AA6" s="16"/>
-      <c r="AB6" s="17"/>
-      <c r="AC6" s="15" t="s">
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="27"/>
+      <c r="AB6" s="28"/>
+      <c r="AC6" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="AD6" s="16"/>
-      <c r="AE6" s="16"/>
-      <c r="AF6" s="16"/>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="16"/>
-      <c r="AI6" s="16"/>
-      <c r="AJ6" s="16"/>
-      <c r="AK6" s="16"/>
-      <c r="AL6" s="16"/>
-      <c r="AM6" s="16"/>
-      <c r="AN6" s="17"/>
+      <c r="AD6" s="27"/>
+      <c r="AE6" s="27"/>
+      <c r="AF6" s="27"/>
+      <c r="AG6" s="27"/>
+      <c r="AH6" s="27"/>
+      <c r="AI6" s="27"/>
+      <c r="AJ6" s="27"/>
+      <c r="AK6" s="27"/>
+      <c r="AL6" s="27"/>
+      <c r="AM6" s="27"/>
+      <c r="AN6" s="28"/>
       <c r="AO6" s="1"/>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.3">
@@ -1084,20 +1085,20 @@
       <c r="B7" s="2"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="23"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="36"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
@@ -1129,20 +1130,20 @@
       <c r="B8" s="2"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="42"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="24"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
@@ -1173,34 +1174,34 @@
       <c r="B9" s="2"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="36" t="s">
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
-      <c r="T9" s="37"/>
-      <c r="U9" s="37"/>
-      <c r="V9" s="37"/>
-      <c r="W9" s="37"/>
-      <c r="X9" s="37"/>
-      <c r="Y9" s="37"/>
-      <c r="Z9" s="37"/>
-      <c r="AA9" s="37"/>
-      <c r="AB9" s="38"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="16"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
       <c r="AE9" s="7"/>
@@ -1347,20 +1348,20 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
@@ -1379,18 +1380,18 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
@@ -1409,20 +1410,20 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
@@ -1441,20 +1442,20 @@
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
@@ -1473,18 +1474,18 @@
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
@@ -1503,20 +1504,20 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
@@ -1535,20 +1536,20 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -1567,20 +1568,20 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
@@ -1599,20 +1600,20 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
@@ -1631,20 +1632,20 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
@@ -1663,20 +1664,20 @@
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
@@ -1695,20 +1696,20 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
@@ -1723,133 +1724,115 @@
       <c r="AB24" s="2"/>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
     </row>
     <row r="33" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="E9:P9"/>
-    <mergeCell ref="Q9:AB9"/>
-    <mergeCell ref="E13:P13"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E2:P2"/>
-    <mergeCell ref="E8:P8"/>
-    <mergeCell ref="Q6:AB6"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="C5:Z5"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="AC2:AN2"/>
-    <mergeCell ref="Q2:AB2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G3:H3"/>
+  <mergeCells count="35">
     <mergeCell ref="AC6:AN6"/>
     <mergeCell ref="E6:P6"/>
     <mergeCell ref="E7:P7"/>
@@ -1866,6 +1849,25 @@
     <mergeCell ref="AC5:AN5"/>
     <mergeCell ref="AA5:AB5"/>
     <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="C5:Z5"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="AC2:AN2"/>
+    <mergeCell ref="Q2:AB2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="E9:P9"/>
+    <mergeCell ref="Q9:AB9"/>
+    <mergeCell ref="E13:P13"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E2:P2"/>
+    <mergeCell ref="E8:P8"/>
+    <mergeCell ref="Q6:AB6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>